<commit_message>
code is ready for production
</commit_message>
<xml_diff>
--- a/BD/FLUXO.xlsx
+++ b/BD/FLUXO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perna\Desktop\STALLANTIS\VIAJANTE\Viajante\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B51766B-45EE-4386-B82F-036A2CA68236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B75DB6-29A2-436D-9EC7-1BCB132DB5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-2445" windowWidth="21840" windowHeight="13020" xr2:uid="{560AD881-1239-4AD1-960A-2C71473C6A4C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{560AD881-1239-4AD1-960A-2C71473C6A4C}"/>
   </bookViews>
   <sheets>
     <sheet name="FLUXOS" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>COD FLUXO</t>
   </si>
@@ -99,13 +99,19 @@
   </si>
   <si>
     <t>JAT</t>
+  </si>
+  <si>
+    <t>32045/43513</t>
+  </si>
+  <si>
+    <t>KOSTAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +123,14 @@
       <b/>
       <sz val="8"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -163,12 +177,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -451,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90B9044-5A84-4453-A4AB-9D3FAB58BBA5}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -549,6 +566,47 @@
         <v>19</v>
       </c>
     </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>76</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2">
+        <v>800043235</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1080</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C4" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>